<commit_message>
updated results, added today projections
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,20 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3C60A3-1981-4FD1-9499-7D8DBE478F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38C15BA-E537-44E9-A651-C7D68921FF27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
     <sheet name="Archive" sheetId="2" r:id="rId2"/>
+    <sheet name="WL Record" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -77,9 +89,6 @@
     <t>Total Win/Loss</t>
   </si>
   <si>
-    <t>November 4th, 2021</t>
-  </si>
-  <si>
     <t>Philadelphia 76ers</t>
   </si>
   <si>
@@ -131,51 +140,33 @@
     <t>Spread Prediction</t>
   </si>
   <si>
-    <t>Detroit +10</t>
-  </si>
-  <si>
     <t>Brooklyn Nets</t>
   </si>
   <si>
-    <t>Orlando +3.5</t>
-  </si>
-  <si>
     <t>San Antonio Spurs</t>
   </si>
   <si>
     <t>Orlando Magic</t>
   </si>
   <si>
-    <t>Memphis +2</t>
-  </si>
-  <si>
     <t>Memphis Grizzlies</t>
   </si>
   <si>
     <t>Washington Wizards</t>
   </si>
   <si>
-    <t>New York +4</t>
-  </si>
-  <si>
     <t>New York Knicks</t>
   </si>
   <si>
     <t>Milwaukee Bucks</t>
   </si>
   <si>
-    <t>Cleveland +5.5</t>
-  </si>
-  <si>
     <t>Cleveland Cavaliers</t>
   </si>
   <si>
     <t>Toronto Raptors</t>
   </si>
   <si>
-    <t>Minnesota +2.5</t>
-  </si>
-  <si>
     <t>Los Angeles Clippers</t>
   </si>
   <si>
@@ -188,27 +179,18 @@
     <t>Golden State Warriors</t>
   </si>
   <si>
-    <t>Portland -5</t>
-  </si>
-  <si>
     <t>Indiana Pacers</t>
   </si>
   <si>
     <t>Portland Trail Blazers</t>
   </si>
   <si>
-    <t>Charlotte +2</t>
-  </si>
-  <si>
     <t>Charlotte Hornets</t>
   </si>
   <si>
     <t>Sacramento Kings</t>
   </si>
   <si>
-    <t>New Orleans -9.5</t>
-  </si>
-  <si>
     <t>Detroit +1</t>
   </si>
   <si>
@@ -236,19 +218,52 @@
     <t>Minnesota -5</t>
   </si>
   <si>
-    <t>Washington -2</t>
-  </si>
-  <si>
-    <t>Milwaukee -4</t>
-  </si>
-  <si>
-    <t>Toronto -5.5</t>
-  </si>
-  <si>
-    <t>Golden State -9.5</t>
-  </si>
-  <si>
-    <t>Sacramento -2</t>
+    <t>Spread Win</t>
+  </si>
+  <si>
+    <t>Spread Loss</t>
+  </si>
+  <si>
+    <t>Over Win</t>
+  </si>
+  <si>
+    <t>Over Loss</t>
+  </si>
+  <si>
+    <t>NO PLAY</t>
+  </si>
+  <si>
+    <t>Chicago Bulls</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>Spread Win %</t>
+  </si>
+  <si>
+    <t>O/U %</t>
+  </si>
+  <si>
+    <t>Houston +10.5</t>
+  </si>
+  <si>
+    <t>Utah +3.5</t>
+  </si>
+  <si>
+    <t>Philadelphia -3.5</t>
+  </si>
+  <si>
+    <t>Boston +4.5</t>
+  </si>
+  <si>
+    <t>Atlanta +4.5</t>
+  </si>
+  <si>
+    <t>Portland -4.5</t>
   </si>
 </sst>
 </file>
@@ -391,7 +406,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,8 +586,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -687,6 +714,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -732,8 +796,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1089,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1108,7 +1184,7 @@
     <col min="10" max="10" width="14.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1116,7 +1192,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1140,292 +1216,229 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
+        <v>52</v>
+      </c>
+      <c r="B2">
+        <v>-10.5</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E2">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H2">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I2">
-        <v>210.5</v>
-      </c>
-      <c r="J2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>-3.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>39</v>
-      </c>
       <c r="E3">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H3">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I3">
         <v>213.5</v>
       </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>207</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>71</v>
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>-3.5</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="E4">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="G4">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H4">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="I4">
-        <v>220.5</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+      <c r="J4">
+        <v>215</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>72</v>
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>-4.5</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="E5">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="G5">
+        <v>103</v>
+      </c>
+      <c r="H5">
+        <v>204</v>
+      </c>
+      <c r="I5">
+        <v>215.5</v>
+      </c>
+      <c r="J5">
+        <v>204</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>-4.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6">
         <v>110</v>
       </c>
-      <c r="H5">
-        <v>221</v>
-      </c>
-      <c r="I5">
-        <v>217</v>
-      </c>
-      <c r="J5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6">
-        <v>101</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="H6">
+        <v>219</v>
+      </c>
+      <c r="I6">
+        <v>224.5</v>
+      </c>
+      <c r="J6">
+        <v>219</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>-4.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
         <v>49</v>
       </c>
-      <c r="G6">
-        <v>102</v>
-      </c>
-      <c r="H6">
-        <v>203</v>
-      </c>
-      <c r="I6">
-        <v>204.5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>52</v>
-      </c>
       <c r="G7">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="H7">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="I7">
-        <v>216.5</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>219.5</v>
+      </c>
+      <c r="J7">
+        <v>224</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8">
-        <v>106</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8">
-        <v>101</v>
-      </c>
-      <c r="H8">
-        <v>207</v>
-      </c>
-      <c r="I8">
-        <v>214.5</v>
-      </c>
-      <c r="J8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9">
-        <v>109</v>
-      </c>
-      <c r="F9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9">
-        <v>115</v>
-      </c>
-      <c r="H9">
-        <v>224</v>
-      </c>
-      <c r="I9">
-        <v>234.5</v>
-      </c>
-      <c r="J9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
         <v>58</v>
-      </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10">
-        <v>116</v>
-      </c>
-      <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10">
-        <v>113</v>
-      </c>
-      <c r="H10">
-        <v>229</v>
-      </c>
-      <c r="I10">
-        <v>223</v>
-      </c>
-      <c r="J10" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1435,15 +1448,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.1796875" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -1503,283 +1517,1584 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6">
+        <v>104</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="6">
+        <v>107</v>
+      </c>
+      <c r="F2" s="6">
+        <f t="shared" ref="F2:F12" si="0">SUM(J2 - L2)</f>
+        <v>8</v>
+      </c>
+      <c r="G2" s="6">
+        <v>5.5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="6">
+        <v>112</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="6">
+        <v>104</v>
+      </c>
+      <c r="M2" s="6">
+        <f t="shared" ref="M2:M12" si="1">SUM(J2+L2)</f>
+        <v>216</v>
+      </c>
+      <c r="N2" s="6">
+        <v>216.5</v>
+      </c>
+      <c r="O2" s="6">
+        <f t="shared" ref="O2:O12" si="2">SUM(C2+E2)</f>
+        <v>211</v>
+      </c>
+      <c r="P2" s="7" t="str">
+        <f t="shared" ref="P2:P12" si="3">IF(M2&lt;N2,"UNDER","OVER")</f>
+        <v>UNDER</v>
+      </c>
+      <c r="Q2" s="6" t="str">
+        <f t="shared" ref="Q2:Q12" si="4">IF(O2&lt;N2,"UNDER","OVER")</f>
+        <v>UNDER</v>
+      </c>
+      <c r="R2" s="9" t="str">
+        <f t="shared" ref="R2:R12" si="5">IF(P2=Q2,"WIN","LOSS")</f>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6">
+        <v>98</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="6">
+        <v>111</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="6">
+        <v>112</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="6">
+        <v>112</v>
+      </c>
+      <c r="M3" s="6">
+        <f t="shared" si="1"/>
+        <v>224</v>
+      </c>
+      <c r="N3" s="6">
+        <v>216</v>
+      </c>
+      <c r="O3" s="6">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="P3" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q3" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R3" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="6">
+        <v>92</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="6">
+        <v>79</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>7</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="6">
+        <v>108</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="6">
+        <v>111</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" si="1"/>
+        <v>219</v>
+      </c>
+      <c r="N4" s="6">
+        <v>213</v>
+      </c>
+      <c r="O4" s="6">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
+      <c r="P4" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q4" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R4" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="6">
+        <v>98</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E5" s="6">
+        <v>103</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="G5" s="6">
+        <v>-2.5</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="6">
+        <v>102</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="6">
+        <v>114</v>
+      </c>
+      <c r="M5" s="6">
+        <f t="shared" si="1"/>
+        <v>216</v>
+      </c>
+      <c r="N5" s="6">
+        <v>215.5</v>
+      </c>
+      <c r="O5" s="6">
+        <f t="shared" si="2"/>
+        <v>201</v>
+      </c>
+      <c r="P5" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q5" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R5" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="6">
+        <v>109</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="6">
+        <v>100</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="G6" s="6">
+        <v>-3.5</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="6">
+        <v>98</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="6">
+        <v>108</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="N6" s="6">
+        <v>212</v>
+      </c>
+      <c r="O6" s="6">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="P6" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q6" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R6" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="6">
+        <v>108</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6">
+        <v>117</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G7" s="6">
+        <v>-4.5</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="6">
+        <v>108</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="6">
+        <v>102</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="N7" s="6">
+        <v>222</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="P7" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q7" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>OVER</v>
+      </c>
+      <c r="R7" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="6">
+        <v>106</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="6">
+        <v>108</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>-27</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="6">
+        <v>90</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="6">
+        <v>117</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="1"/>
+        <v>207</v>
+      </c>
+      <c r="N8" s="6">
+        <v>215</v>
+      </c>
+      <c r="O8" s="6">
+        <f t="shared" si="2"/>
+        <v>214</v>
+      </c>
+      <c r="P8" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q8" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R8" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="6">
+        <v>126</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="6">
+        <v>115</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="G9" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="6">
+        <v>95</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="6">
+        <v>100</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="N9" s="6">
+        <v>212.5</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="2"/>
+        <v>241</v>
+      </c>
+      <c r="P9" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q9" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>OVER</v>
+      </c>
+      <c r="R9" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="6">
+        <v>109</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="6">
+        <v>108</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="G10" s="6">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="6">
+        <v>99</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="6">
+        <v>109</v>
+      </c>
+      <c r="M10" s="6">
+        <f t="shared" si="1"/>
+        <v>208</v>
+      </c>
+      <c r="N10" s="6">
+        <v>217.5</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" si="2"/>
+        <v>217</v>
+      </c>
+      <c r="P10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q10" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R10" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="6">
+        <v>92</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="6">
+        <v>114</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G11" s="6">
+        <v>-6</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="6">
+        <v>119</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="6">
+        <v>102</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="1"/>
+        <v>221</v>
+      </c>
+      <c r="N11" s="6">
+        <v>226.5</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="2"/>
+        <v>206</v>
+      </c>
+      <c r="P11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q11" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R11" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>44503</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="6">
+        <v>99</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="6">
+        <v>112</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="G12" s="6">
+        <v>-6</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="6">
+        <v>106</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="6">
+        <v>114</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="N12" s="6">
+        <v>219</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="2"/>
+        <v>211</v>
+      </c>
+      <c r="P12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q12" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R12" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <v>44504</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>109</v>
+      </c>
+      <c r="D13" t="s">
         <v>19</v>
       </c>
+      <c r="E13">
+        <v>98</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>-5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13">
+        <v>109</v>
+      </c>
+      <c r="K13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13">
+        <v>98</v>
+      </c>
+      <c r="M13">
+        <v>207</v>
+      </c>
+      <c r="N13">
+        <v>208</v>
+      </c>
+      <c r="O13">
+        <v>207</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <v>44504</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>116</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14">
+        <v>98</v>
+      </c>
+      <c r="F14">
+        <v>-2</v>
+      </c>
+      <c r="G14">
+        <v>-6.5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14">
+        <v>104</v>
+      </c>
+      <c r="K14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L14">
+        <v>106</v>
+      </c>
+      <c r="M14">
+        <v>210</v>
+      </c>
+      <c r="N14">
+        <v>214.5</v>
+      </c>
+      <c r="O14">
+        <v>214</v>
+      </c>
+      <c r="P14" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>44504</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <v>95</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <v>78</v>
+      </c>
+      <c r="F15">
+        <v>-9</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15">
+        <v>103</v>
+      </c>
+      <c r="K15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15">
+        <v>112</v>
+      </c>
+      <c r="M15">
+        <v>215</v>
+      </c>
+      <c r="N15">
+        <v>219.5</v>
+      </c>
+      <c r="O15">
+        <v>173</v>
+      </c>
+      <c r="P15" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>44504</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <v>123</v>
+      </c>
+      <c r="F16">
+        <v>-7</v>
+      </c>
+      <c r="G16">
+        <v>-10.5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16">
+        <v>101</v>
+      </c>
+      <c r="K16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16">
+        <v>108</v>
+      </c>
+      <c r="M16">
+        <v>209</v>
+      </c>
+      <c r="N16">
+        <v>218</v>
+      </c>
+      <c r="O16">
+        <v>234</v>
+      </c>
+      <c r="P16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>31</v>
+      </c>
+      <c r="R16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>44504</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>107</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17">
+        <v>104</v>
+      </c>
+      <c r="F17">
+        <v>-15</v>
+      </c>
+      <c r="G17">
+        <v>-10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17">
+        <v>98</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17">
+        <v>113</v>
+      </c>
+      <c r="M17">
+        <v>211</v>
+      </c>
+      <c r="N17">
+        <v>214</v>
+      </c>
+      <c r="O17">
+        <v>211</v>
+      </c>
+      <c r="P17" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>22</v>
+      </c>
+      <c r="R17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2">
+        <v>96</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2">
+        <v>90</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" ref="F18:F26" si="6">SUM(J18 - L18)</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="2">
+        <v>101</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="2">
+        <v>100</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" ref="M18:M26" si="7">SUM(J18+L18)</f>
+        <v>201</v>
+      </c>
+      <c r="N18" s="2">
+        <v>210.5</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" ref="O18:O26" si="8">SUM(C18+E18)</f>
+        <v>186</v>
+      </c>
+      <c r="P18" s="3" t="str">
+        <f t="shared" ref="P18:P26" si="9">IF(M18&lt;N18,"UNDER","OVER")</f>
+        <v>UNDER</v>
+      </c>
+      <c r="Q18" s="2" t="str">
+        <f t="shared" ref="Q18:Q26" si="10">IF(O18&lt;N18,"UNDER","OVER")</f>
+        <v>UNDER</v>
+      </c>
+      <c r="R18" s="2" t="str">
+        <f t="shared" ref="R18:R26" si="11">IF(P18=Q18,"WIN","LOSS")</f>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <v>102</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="2">
+        <v>89</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="2">
+        <v>105</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="2">
+        <v>107</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="7"/>
+        <v>212</v>
+      </c>
+      <c r="N19" s="2">
+        <v>213.5</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="8"/>
+        <v>191</v>
+      </c>
+      <c r="P19" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q19" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R19" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2">
+        <v>87</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="2">
+        <v>115</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-2</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="2">
+        <v>113</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L20" s="2">
+        <v>108</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="7"/>
+        <v>221</v>
+      </c>
+      <c r="N20" s="2">
+        <v>220.5</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="8"/>
+        <v>202</v>
+      </c>
+      <c r="P20" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q20" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R20" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2">
+        <v>113</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="2">
+        <v>98</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="2">
+        <v>-4</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" s="2">
+        <v>111</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" s="2">
+        <v>110</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="7"/>
+        <v>221</v>
+      </c>
+      <c r="N21" s="2">
+        <v>217</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="8"/>
+        <v>211</v>
+      </c>
+      <c r="P21" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q21" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R21" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2">
+        <v>102</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="2">
+        <v>101</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="G22" s="2">
+        <v>-5.5</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="2">
+        <v>101</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L22" s="2">
+        <v>102</v>
+      </c>
+      <c r="M22" s="2">
+        <f t="shared" si="7"/>
+        <v>203</v>
+      </c>
+      <c r="N22" s="2">
+        <v>204.5</v>
+      </c>
+      <c r="O22" s="2">
+        <f t="shared" si="8"/>
+        <v>203</v>
+      </c>
+      <c r="P22" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q22" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R22" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2">
+        <v>104</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="2">
+        <v>84</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J23" s="2">
+        <v>100</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L23" s="2">
+        <v>105</v>
+      </c>
+      <c r="M23" s="2">
+        <f t="shared" si="7"/>
+        <v>205</v>
+      </c>
+      <c r="N23" s="2">
+        <v>216.5</v>
+      </c>
+      <c r="O23" s="2">
+        <f t="shared" si="8"/>
+        <v>188</v>
+      </c>
+      <c r="P23" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q23" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R23" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="2">
+        <v>85</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="2">
+        <v>126</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="G24" s="2">
+        <v>-9.5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="2">
+        <v>106</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L24" s="2">
+        <v>101</v>
+      </c>
+      <c r="M24" s="2">
+        <f t="shared" si="7"/>
+        <v>207</v>
+      </c>
+      <c r="N24" s="2">
+        <v>214.5</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="8"/>
+        <v>211</v>
+      </c>
+      <c r="P24" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q24" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R24" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="2">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2">
+        <v>110</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="6"/>
+        <v>-6</v>
+      </c>
+      <c r="G25" s="2">
+        <v>-5</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="2">
+        <v>109</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L25" s="2">
+        <v>115</v>
+      </c>
+      <c r="M25" s="2">
+        <f t="shared" si="7"/>
+        <v>224</v>
+      </c>
+      <c r="N25" s="2">
+        <v>234.5</v>
+      </c>
+      <c r="O25" s="2">
+        <f t="shared" si="8"/>
+        <v>216</v>
+      </c>
+      <c r="P25" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q25" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R25" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>44505</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="2">
+        <v>110</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="2">
+        <v>140</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="G26" s="2">
+        <v>-2</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" s="2">
+        <v>116</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26" s="2">
+        <v>113</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="7"/>
+        <v>229</v>
+      </c>
+      <c r="N26" s="2">
+        <v>223</v>
+      </c>
+      <c r="O26" s="2">
+        <f t="shared" si="8"/>
+        <v>250</v>
+      </c>
+      <c r="P26" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q26" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R26" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDBD52-5F97-49F2-81E9-5AECCF07C193}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="3" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>COUNTIF(Archive!$H2:H111,"WIN")</f>
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIF(Archive!$H2:H111,"LOSS")</f>
+        <v>14</v>
+      </c>
       <c r="C2">
-        <v>109</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
+        <f>ROUND(SUM(A2/(A2+B2)),3)</f>
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF(Archive!$R2:R111,"WIN")</f>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>98</v>
-      </c>
-      <c r="F2">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>-5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2">
-        <v>109</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2">
-        <v>98</v>
-      </c>
-      <c r="M2">
-        <v>207</v>
-      </c>
-      <c r="N2">
-        <v>208</v>
-      </c>
-      <c r="O2">
-        <v>207</v>
-      </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3">
-        <v>116</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3">
-        <v>98</v>
-      </c>
-      <c r="F3">
-        <v>-2</v>
-      </c>
-      <c r="G3">
-        <v>-6.5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3">
-        <v>104</v>
-      </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3">
-        <v>106</v>
-      </c>
-      <c r="M3">
-        <v>210</v>
-      </c>
-      <c r="N3">
-        <v>214.5</v>
-      </c>
-      <c r="O3">
-        <v>214</v>
-      </c>
-      <c r="P3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>95</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4">
-        <v>78</v>
-      </c>
-      <c r="F4">
-        <v>-9</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4">
-        <v>103</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4">
-        <v>112</v>
-      </c>
-      <c r="M4">
-        <v>215</v>
-      </c>
-      <c r="N4">
-        <v>219.5</v>
-      </c>
-      <c r="O4">
-        <v>173</v>
-      </c>
-      <c r="P4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5">
-        <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>123</v>
-      </c>
-      <c r="F5">
-        <v>-7</v>
-      </c>
-      <c r="G5">
-        <v>-10.5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5">
-        <v>101</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5">
-        <v>108</v>
-      </c>
-      <c r="M5">
-        <v>209</v>
-      </c>
-      <c r="N5">
-        <v>218</v>
-      </c>
-      <c r="O5">
-        <v>234</v>
-      </c>
-      <c r="P5" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <v>107</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6">
-        <v>104</v>
-      </c>
-      <c r="F6">
-        <v>-15</v>
-      </c>
-      <c r="G6">
-        <v>-10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6">
-        <v>98</v>
-      </c>
-      <c r="K6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6">
-        <v>113</v>
-      </c>
-      <c r="M6">
-        <v>211</v>
-      </c>
-      <c r="N6">
-        <v>214</v>
-      </c>
-      <c r="O6">
-        <v>211</v>
-      </c>
-      <c r="P6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>23</v>
-      </c>
-      <c r="R6" t="s">
-        <v>21</v>
+        <f>COUNTIF(Archive!$R2:R111,"LOSS")</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update results and predictions
11/8/2021
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03206A11-8433-46EC-AA85-EF4CEE022525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A08654-28A9-4244-8538-DCB8E42ACFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -227,28 +227,28 @@
     <t>Vegas Line(Home)</t>
   </si>
   <si>
-    <t>Toronto +4</t>
-  </si>
-  <si>
-    <t>Orlando +13</t>
-  </si>
-  <si>
-    <t>Washington +3</t>
-  </si>
-  <si>
-    <t>Oklahoma City +4</t>
-  </si>
-  <si>
-    <t>New York -7.5</t>
-  </si>
-  <si>
-    <t>Sacramento -1.5</t>
-  </si>
-  <si>
-    <t>Houston +10</t>
-  </si>
-  <si>
-    <t>Charlotte +5</t>
+    <t>New York +4.5</t>
+  </si>
+  <si>
+    <t>New Orleans +9</t>
+  </si>
+  <si>
+    <t>Atlanta +3.5</t>
+  </si>
+  <si>
+    <t>Charlotte +2.5</t>
+  </si>
+  <si>
+    <t>Chicago -2</t>
+  </si>
+  <si>
+    <t>Memphis -2</t>
+  </si>
+  <si>
+    <t>Miami -2</t>
+  </si>
+  <si>
+    <t>Sacramento +2.5</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1204,144 +1204,144 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>4</v>
+        <v>-4.5</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D2">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="F2">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="G2">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="H2">
-        <v>209.5</v>
+        <v>210.5</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-7.5</v>
+        <v>-2</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D3">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F3">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G3">
+        <v>208</v>
+      </c>
+      <c r="H3">
         <v>216</v>
       </c>
-      <c r="H3">
-        <v>209.5</v>
-      </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>13</v>
+        <v>-6</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D4">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F4">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="G4">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H4">
-        <v>212</v>
+        <v>218.5</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>-1.5</v>
+        <v>-9</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="F5">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="G5">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="H5">
-        <v>223</v>
+        <v>210.5</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D6">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="F6">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G6">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="H6">
-        <v>221.5</v>
+        <v>205</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -1349,28 +1349,28 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>4</v>
+        <v>-3.5</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F7">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G7">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="H7">
-        <v>211.5</v>
+        <v>221.5</v>
       </c>
       <c r="I7" t="s">
         <v>22</v>
@@ -1378,60 +1378,60 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>13</v>
+        <v>2.5</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F8">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="G8">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="H8">
-        <v>220</v>
+        <v>222.5</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>-5</v>
+        <v>-2.5</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
       </c>
       <c r="D9">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G9">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="H9">
-        <v>222.5</v>
+        <v>224.5</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1441,16 +1441,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:R32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -2488,7 +2488,7 @@
         <v>90</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" ref="F18:F32" si="6">SUM(J18 - L18)</f>
+        <f t="shared" ref="F18:F40" si="6">SUM(J18 - L18)</f>
         <v>1</v>
       </c>
       <c r="G18" s="2">
@@ -2510,26 +2510,26 @@
         <v>100</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" ref="M18:M32" si="7">SUM(J18+L18)</f>
+        <f t="shared" ref="M18:M40" si="7">SUM(J18+L18)</f>
         <v>201</v>
       </c>
       <c r="N18" s="2">
         <v>210.5</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" ref="O18:O32" si="8">SUM(C18+E18)</f>
+        <f t="shared" ref="O18:O40" si="8">SUM(C18+E18)</f>
         <v>186</v>
       </c>
       <c r="P18" s="3" t="str">
-        <f t="shared" ref="P18:P32" si="9">IF(M18&lt;N18,"UNDER","OVER")</f>
+        <f t="shared" ref="P18:P40" si="9">IF(M18&lt;N18,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="Q18" s="2" t="str">
-        <f t="shared" ref="Q18:Q32" si="10">IF(O18&lt;N18,"UNDER","OVER")</f>
+        <f t="shared" ref="Q18:Q40" si="10">IF(O18&lt;N18,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="R18" s="2" t="str">
-        <f t="shared" ref="R18:R32" si="11">IF(P18=Q18,"WIN","LOSS")</f>
+        <f t="shared" ref="R18:R40" si="11">IF(P18=Q18,"WIN","LOSS")</f>
         <v>WIN</v>
       </c>
     </row>
@@ -3397,6 +3397,502 @@
         <v>UNDER</v>
       </c>
       <c r="R32" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A33" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="12">
+        <v>116</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="12">
+        <v>103</v>
+      </c>
+      <c r="F33" s="12">
+        <f t="shared" si="6"/>
+        <v>-4</v>
+      </c>
+      <c r="G33" s="12">
+        <v>4</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33" s="12">
+        <v>99</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L33" s="12">
+        <v>103</v>
+      </c>
+      <c r="M33" s="12">
+        <f t="shared" si="7"/>
+        <v>202</v>
+      </c>
+      <c r="N33" s="12">
+        <v>209.5</v>
+      </c>
+      <c r="O33" s="12">
+        <f t="shared" si="8"/>
+        <v>219</v>
+      </c>
+      <c r="P33" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q33" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R33" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A34" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="12">
+        <v>126</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="12">
+        <v>109</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" si="6"/>
+        <v>-12</v>
+      </c>
+      <c r="G34" s="12">
+        <v>-7.5</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J34" s="12">
+        <v>102</v>
+      </c>
+      <c r="K34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L34" s="12">
+        <v>114</v>
+      </c>
+      <c r="M34" s="12">
+        <f t="shared" si="7"/>
+        <v>216</v>
+      </c>
+      <c r="N34" s="12">
+        <v>209.5</v>
+      </c>
+      <c r="O34" s="12">
+        <f t="shared" si="8"/>
+        <v>235</v>
+      </c>
+      <c r="P34" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q34" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R34" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A35" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="12">
+        <v>100</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="12">
+        <v>107</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G35" s="12">
+        <v>13</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J35" s="12">
+        <v>107</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L35" s="12">
+        <v>105</v>
+      </c>
+      <c r="M35" s="12">
+        <f t="shared" si="7"/>
+        <v>212</v>
+      </c>
+      <c r="N35" s="12">
+        <v>212</v>
+      </c>
+      <c r="O35" s="12">
+        <f t="shared" si="8"/>
+        <v>207</v>
+      </c>
+      <c r="P35" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q35" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R35" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A36" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="12">
+        <v>94</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="12">
+        <v>91</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="6"/>
+        <v>-8</v>
+      </c>
+      <c r="G36" s="12">
+        <v>-1.5</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36" s="12">
+        <v>109</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="12">
+        <v>117</v>
+      </c>
+      <c r="M36" s="12">
+        <f t="shared" si="7"/>
+        <v>226</v>
+      </c>
+      <c r="N36" s="12">
+        <v>223</v>
+      </c>
+      <c r="O36" s="12">
+        <f t="shared" si="8"/>
+        <v>185</v>
+      </c>
+      <c r="P36" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q36" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R36" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A37" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="12">
+        <v>94</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="12">
+        <v>101</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="12">
+        <v>3</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J37" s="12">
+        <v>107</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L37" s="12">
+        <v>107</v>
+      </c>
+      <c r="M37" s="12">
+        <f t="shared" si="7"/>
+        <v>214</v>
+      </c>
+      <c r="N37" s="12">
+        <v>221.5</v>
+      </c>
+      <c r="O37" s="12">
+        <f t="shared" si="8"/>
+        <v>195</v>
+      </c>
+      <c r="P37" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q37" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R37" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A38" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="12">
+        <v>94</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="12">
+        <v>99</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="G38" s="12">
+        <v>4</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" s="12">
+        <v>103</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="L38" s="12">
+        <v>102</v>
+      </c>
+      <c r="M38" s="12">
+        <f t="shared" si="7"/>
+        <v>205</v>
+      </c>
+      <c r="N38" s="12">
+        <v>211.5</v>
+      </c>
+      <c r="O38" s="12">
+        <f t="shared" si="8"/>
+        <v>193</v>
+      </c>
+      <c r="P38" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q38" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R38" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A39" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="12">
+        <v>107</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="12">
+        <v>120</v>
+      </c>
+      <c r="F39" s="12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="12">
+        <v>13</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="12">
+        <v>102</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L39" s="12">
+        <v>102</v>
+      </c>
+      <c r="M39" s="12">
+        <f t="shared" si="7"/>
+        <v>204</v>
+      </c>
+      <c r="N39" s="12">
+        <v>220</v>
+      </c>
+      <c r="O39" s="12">
+        <f t="shared" si="8"/>
+        <v>227</v>
+      </c>
+      <c r="P39" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q39" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R39" s="14" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A40" s="11">
+        <v>44507</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="12">
+        <v>106</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="12">
+        <v>120</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="G40" s="12">
+        <v>-5</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J40" s="12">
+        <v>119</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L40" s="12">
+        <v>100</v>
+      </c>
+      <c r="M40" s="12">
+        <f t="shared" si="7"/>
+        <v>219</v>
+      </c>
+      <c r="N40" s="12">
+        <v>222.5</v>
+      </c>
+      <c r="O40" s="12">
+        <f t="shared" si="8"/>
+        <v>226</v>
+      </c>
+      <c r="P40" s="13" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q40" s="12" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R40" s="14" t="str">
         <f t="shared" si="11"/>
         <v>LOSS</v>
       </c>
@@ -3410,8 +3906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDBD52-5F97-49F2-81E9-5AECCF07C193}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3443,23 +3939,23 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>COUNTIF(Archive!$H2:H111,"WIN")</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <f>COUNTIF(Archive!$H2:H111,"LOSS")</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <f>ROUND(SUM(A2/(A2+B2)),3)</f>
-        <v>0.51700000000000002</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="D2">
         <f>COUNTIF(Archive!$R2:R111,"WIN")</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <f>COUNTIF(Archive!$R2:R111,"LOSS")</f>
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update projections + add jupyter
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55AE199-6564-45E1-94CE-E5472C263F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC55CD37-ADF5-4A42-B0A8-F2FE808856D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -227,13 +227,43 @@
     <t>Vegas Line(Home)</t>
   </si>
   <si>
-    <t>Phildaelphia +6.5</t>
-  </si>
-  <si>
-    <t>Atlanta +8</t>
-  </si>
-  <si>
-    <t>Portland +3</t>
+    <t>Cleveland +3</t>
+  </si>
+  <si>
+    <t>Orlando +9</t>
+  </si>
+  <si>
+    <t>Boston - 2</t>
+  </si>
+  <si>
+    <t>Houston -3.5</t>
+  </si>
+  <si>
+    <t>New York -3</t>
+  </si>
+  <si>
+    <t>Chicago -3</t>
+  </si>
+  <si>
+    <t>Charlotte +4.5</t>
+  </si>
+  <si>
+    <t>New Orleans -4.5</t>
+  </si>
+  <si>
+    <t>Sacramento - Pick</t>
+  </si>
+  <si>
+    <t>Indiana - 3</t>
+  </si>
+  <si>
+    <t>Portland +6</t>
+  </si>
+  <si>
+    <t>Minnesota +7</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers +4.5</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1189,28 +1219,28 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="F2">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G2">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H2">
-        <v>220.5</v>
+        <v>211.5</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
@@ -1218,59 +1248,349 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D3">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="F3">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G3">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="H3">
-        <v>221.5</v>
+        <v>209.5</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="B4" t="s">
         <v>66</v>
       </c>
       <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>105</v>
+      </c>
+      <c r="G4">
+        <v>207</v>
+      </c>
+      <c r="H4">
+        <v>209.5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>-3.5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>95</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>106</v>
+      </c>
+      <c r="G5">
+        <v>201</v>
+      </c>
+      <c r="H5">
+        <v>210.5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>-3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>114</v>
+      </c>
+      <c r="G6">
+        <v>220</v>
+      </c>
+      <c r="H6">
+        <v>215.5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>-3.5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7">
+        <v>107</v>
+      </c>
+      <c r="G7">
+        <v>207</v>
+      </c>
+      <c r="H7">
+        <v>213</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>-4.5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>117</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8">
+        <v>115</v>
+      </c>
+      <c r="G8">
+        <v>232</v>
+      </c>
+      <c r="H8">
+        <v>228.5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>-4.5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>97</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9">
+        <v>108</v>
+      </c>
+      <c r="G9">
+        <v>205</v>
+      </c>
+      <c r="H9">
+        <v>211</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>109</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10">
+        <v>104</v>
+      </c>
+      <c r="G10">
+        <v>213</v>
+      </c>
+      <c r="H10">
+        <v>220</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11">
+        <v>96</v>
+      </c>
+      <c r="G11">
+        <v>203</v>
+      </c>
+      <c r="H11">
+        <v>213</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>-6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
         <v>48</v>
       </c>
-      <c r="D4">
-        <v>109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4">
-        <v>102</v>
-      </c>
-      <c r="G4">
-        <v>211</v>
-      </c>
-      <c r="H4">
-        <v>220</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="D12">
+        <v>110</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>111</v>
+      </c>
+      <c r="G12">
+        <v>221</v>
+      </c>
+      <c r="H12">
+        <v>220.5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>-7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>101</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13">
+        <v>106</v>
+      </c>
+      <c r="G13">
+        <v>207</v>
+      </c>
+      <c r="H13">
+        <v>222.5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>4.5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14">
+        <v>104</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14">
+        <v>110</v>
+      </c>
+      <c r="G14">
+        <v>214</v>
+      </c>
+      <c r="H14">
+        <v>214.5</v>
+      </c>
+      <c r="I14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1281,16 +1601,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.1796875" customWidth="1"/>
     <col min="2" max="2" width="18.90625" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -2328,7 +2649,7 @@
         <v>90</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" ref="F18:F48" si="6">SUM(J18 - L18)</f>
+        <f t="shared" ref="F18:F51" si="6">SUM(J18 - L18)</f>
         <v>1</v>
       </c>
       <c r="G18" s="2">
@@ -2350,26 +2671,26 @@
         <v>100</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" ref="M18:M48" si="7">SUM(J18+L18)</f>
+        <f t="shared" ref="M18:M51" si="7">SUM(J18+L18)</f>
         <v>201</v>
       </c>
       <c r="N18" s="2">
         <v>210.5</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" ref="O18:O48" si="8">SUM(C18+E18)</f>
+        <f t="shared" ref="O18:O51" si="8">SUM(C18+E18)</f>
         <v>186</v>
       </c>
       <c r="P18" s="3" t="str">
-        <f t="shared" ref="P18:P48" si="9">IF(M18&lt;N18,"UNDER","OVER")</f>
+        <f t="shared" ref="P18:P51" si="9">IF(M18&lt;N18,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="Q18" s="2" t="str">
-        <f t="shared" ref="Q18:Q48" si="10">IF(O18&lt;N18,"UNDER","OVER")</f>
+        <f t="shared" ref="Q18:Q51" si="10">IF(O18&lt;N18,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="R18" s="2" t="str">
-        <f t="shared" ref="R18:R48" si="11">IF(P18=Q18,"WIN","LOSS")</f>
+        <f t="shared" ref="R18:R51" si="11">IF(P18=Q18,"WIN","LOSS")</f>
         <v>WIN</v>
       </c>
     </row>
@@ -4231,6 +4552,192 @@
       <c r="R48" s="14" t="str">
         <f t="shared" si="11"/>
         <v>WIN</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>44509</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="2">
+        <v>118</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="2">
+        <v>109</v>
+      </c>
+      <c r="F49" s="2">
+        <f t="shared" si="6"/>
+        <v>-7</v>
+      </c>
+      <c r="G49" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J49" s="2">
+        <v>105</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L49" s="2">
+        <v>112</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="7"/>
+        <v>217</v>
+      </c>
+      <c r="N49" s="2">
+        <v>220.5</v>
+      </c>
+      <c r="O49" s="2">
+        <f t="shared" si="8"/>
+        <v>227</v>
+      </c>
+      <c r="P49" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q49" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R49" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>44509</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="2">
+        <v>98</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="2">
+        <v>110</v>
+      </c>
+      <c r="F50" s="2">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G50" s="2">
+        <v>-8</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J50" s="2">
+        <v>112</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L50" s="2">
+        <v>110</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="7"/>
+        <v>222</v>
+      </c>
+      <c r="N50" s="2">
+        <v>221.5</v>
+      </c>
+      <c r="O50" s="2">
+        <f t="shared" si="8"/>
+        <v>208</v>
+      </c>
+      <c r="P50" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q50" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R50" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>44509</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="2">
+        <v>109</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="2">
+        <v>117</v>
+      </c>
+      <c r="F51" s="2">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="G51" s="2">
+        <v>-3</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J51" s="2">
+        <v>109</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="2">
+        <v>102</v>
+      </c>
+      <c r="M51" s="2">
+        <f t="shared" si="7"/>
+        <v>211</v>
+      </c>
+      <c r="N51" s="2">
+        <v>220</v>
+      </c>
+      <c r="O51" s="2">
+        <f t="shared" si="8"/>
+        <v>226</v>
+      </c>
+      <c r="P51" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q51" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R51" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
       </c>
     </row>
   </sheetData>
@@ -4242,7 +4749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDBD52-5F97-49F2-81E9-5AECCF07C193}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -4279,11 +4786,11 @@
       </c>
       <c r="B2">
         <f>COUNTIF(Archive!$H2:H111,"LOSS")</f>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <f>ROUND(SUM(A2/(A2+B2)),3)</f>
-        <v>0.46700000000000003</v>
+        <v>0.438</v>
       </c>
       <c r="D2">
         <f>COUNTIF(Archive!$R2:R111,"WIN")</f>
@@ -4291,11 +4798,11 @@
       </c>
       <c r="E2">
         <f>COUNTIF(Archive!$R2:R111,"LOSS")</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <f>ROUND(SUM(D2/(D2+E2)),3)</f>
-        <v>0.53200000000000003</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed NBA model algo - Updated Projections
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A21DFCF-57C0-49BC-8A38-1884B623D3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B296DBDA-9AF0-4960-A31E-58353F51C850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -233,10 +233,10 @@
     <t>Philadelphia -3</t>
   </si>
   <si>
-    <t>Indiana +9.5</t>
-  </si>
-  <si>
-    <t>Miami +4</t>
+    <t>Utah -9.5</t>
+  </si>
+  <si>
+    <t>Los Angeles Clippers -4</t>
   </si>
 </sst>
 </file>
@@ -1144,14 +1144,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
     <col min="3" max="3" width="19.26953125" customWidth="1"/>
     <col min="4" max="4" width="16.08984375" customWidth="1"/>
     <col min="5" max="5" width="22.453125" customWidth="1"/>
@@ -1201,13 +1201,13 @@
         <v>42</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
       <c r="F2">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G2">
         <v>213</v>
@@ -1259,22 +1259,22 @@
         <v>26</v>
       </c>
       <c r="D4">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="G4">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H4">
         <v>211.5</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -5238,7 +5238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDBD52-5F97-49F2-81E9-5AECCF07C193}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated results and proj 11-14-21
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703AB202-F4CE-4A1F-8572-AFA7955CA1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735BDC1B-1023-4C5B-8174-ACF2EAB33F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="72">
   <si>
     <t>Date</t>
   </si>
@@ -230,25 +230,25 @@
     <t>PUSH</t>
   </si>
   <si>
-    <t>Miami +7</t>
-  </si>
-  <si>
-    <t>Philadelphia +3.5</t>
-  </si>
-  <si>
-    <t>New Orleans +4</t>
-  </si>
-  <si>
-    <t>Washington -4.5</t>
-  </si>
-  <si>
-    <t>Toronto -9.5</t>
-  </si>
-  <si>
-    <t>Cleveland +2.5</t>
-  </si>
-  <si>
-    <t>Los Angeles Clippers -7</t>
+    <t>San Antonio +2.5</t>
+  </si>
+  <si>
+    <t>Milwaukee +1.5</t>
+  </si>
+  <si>
+    <t>Golden State -5</t>
+  </si>
+  <si>
+    <t>Houston +8.5</t>
+  </si>
+  <si>
+    <t>Oklahoma City +9</t>
+  </si>
+  <si>
+    <t>Portland +6.5</t>
+  </si>
+  <si>
+    <t>Los Angeles Clippers -4</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1157,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1204,28 +1204,28 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D2">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F2">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G2">
         <v>213</v>
       </c>
       <c r="H2">
-        <v>214</v>
+        <v>219.5</v>
       </c>
       <c r="I2" t="s">
         <v>22</v>
@@ -1233,115 +1233,115 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-3.5</v>
+        <v>-1.5</v>
       </c>
       <c r="B3" t="s">
         <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D3">
+        <v>111</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
         <v>109</v>
       </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3">
-        <v>110</v>
-      </c>
       <c r="G3">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H3">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D4">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F4">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G4">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H4">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D5">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F5">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G5">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="H5">
-        <v>203.5</v>
+        <v>221</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>-9.5</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="F6">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G6">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="H6">
-        <v>201.5</v>
+        <v>214.5</v>
       </c>
       <c r="I6" t="s">
         <v>22</v>
@@ -1349,45 +1349,45 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>2.5</v>
+        <v>-6.5</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="F7">
         <v>104</v>
       </c>
       <c r="G7">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H7">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>-7</v>
+        <v>-4</v>
       </c>
       <c r="B8" t="s">
         <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="D8">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
@@ -1396,10 +1396,10 @@
         <v>109</v>
       </c>
       <c r="G8">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="H8">
-        <v>220.5</v>
+        <v>218</v>
       </c>
       <c r="I8" t="s">
         <v>22</v>
@@ -1412,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R78"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:R78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I69" sqref="I69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2460,7 +2460,7 @@
         <v>90</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" ref="F18:F78" si="6">SUM(J18 - L18)</f>
+        <f t="shared" ref="F18:F81" si="6">SUM(J18 - L18)</f>
         <v>1</v>
       </c>
       <c r="G18" s="2">
@@ -2482,26 +2482,26 @@
         <v>100</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" ref="M18:M78" si="7">SUM(J18+L18)</f>
+        <f t="shared" ref="M18:M81" si="7">SUM(J18+L18)</f>
         <v>201</v>
       </c>
       <c r="N18" s="2">
         <v>210.5</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" ref="O18:O78" si="8">SUM(C18+E18)</f>
+        <f t="shared" ref="O18:O81" si="8">SUM(C18+E18)</f>
         <v>186</v>
       </c>
       <c r="P18" s="3" t="str">
-        <f t="shared" ref="P18:P78" si="9">IF(M18&lt;N18,"UNDER","OVER")</f>
+        <f t="shared" ref="P18:P81" si="9">IF(M18&lt;N18,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="Q18" s="2" t="str">
-        <f t="shared" ref="Q18:Q78" si="10">IF(O18&lt;N18,"UNDER","OVER")</f>
+        <f t="shared" ref="Q18:Q81" si="10">IF(O18&lt;N18,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="R18" s="2" t="str">
-        <f t="shared" ref="R18:R78" si="11">IF(P18=Q18,"WIN","LOSS")</f>
+        <f t="shared" ref="R18:R81" si="11">IF(P18=Q18,"WIN","LOSS")</f>
         <v>WIN</v>
       </c>
     </row>
@@ -6223,6 +6223,440 @@
       <c r="R78" s="14" t="str">
         <f t="shared" si="11"/>
         <v>WIN</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C79" s="2">
+        <v>111</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="2">
+        <v>105</v>
+      </c>
+      <c r="F79" s="2">
+        <f t="shared" si="6"/>
+        <v>-5</v>
+      </c>
+      <c r="G79" s="2">
+        <v>-7</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J79" s="2">
+        <v>104</v>
+      </c>
+      <c r="K79" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L79" s="2">
+        <v>109</v>
+      </c>
+      <c r="M79" s="2">
+        <f t="shared" si="7"/>
+        <v>213</v>
+      </c>
+      <c r="N79" s="2">
+        <v>214</v>
+      </c>
+      <c r="O79" s="2">
+        <f t="shared" si="8"/>
+        <v>216</v>
+      </c>
+      <c r="P79" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q79" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R79" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="2">
+        <v>113</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80" s="2">
+        <v>118</v>
+      </c>
+      <c r="F80" s="2">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="G80" s="2">
+        <v>-3.5</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J80" s="2">
+        <v>109</v>
+      </c>
+      <c r="K80" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L80" s="2">
+        <v>110</v>
+      </c>
+      <c r="M80" s="2">
+        <f t="shared" si="7"/>
+        <v>219</v>
+      </c>
+      <c r="N80" s="2">
+        <v>214</v>
+      </c>
+      <c r="O80" s="2">
+        <f t="shared" si="8"/>
+        <v>231</v>
+      </c>
+      <c r="P80" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q80" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>OVER</v>
+      </c>
+      <c r="R80" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C81" s="2">
+        <v>101</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E81" s="2">
+        <v>112</v>
+      </c>
+      <c r="F81" s="2">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="G81" s="2">
+        <v>4</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J81" s="2">
+        <v>111</v>
+      </c>
+      <c r="K81" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L81" s="2">
+        <v>108</v>
+      </c>
+      <c r="M81" s="2">
+        <f t="shared" si="7"/>
+        <v>219</v>
+      </c>
+      <c r="N81" s="2">
+        <v>218</v>
+      </c>
+      <c r="O81" s="2">
+        <f t="shared" si="8"/>
+        <v>213</v>
+      </c>
+      <c r="P81" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q81" s="2" t="str">
+        <f t="shared" si="10"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R81" s="2" t="str">
+        <f t="shared" si="11"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="2">
+        <v>104</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E82" s="2">
+        <v>92</v>
+      </c>
+      <c r="F82" s="2">
+        <f t="shared" ref="F82:F85" si="12">SUM(J82 - L82)</f>
+        <v>10</v>
+      </c>
+      <c r="G82" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J82" s="2">
+        <v>107</v>
+      </c>
+      <c r="K82" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L82" s="2">
+        <v>97</v>
+      </c>
+      <c r="M82" s="2">
+        <f t="shared" ref="M82:M85" si="13">SUM(J82+L82)</f>
+        <v>204</v>
+      </c>
+      <c r="N82" s="2">
+        <v>203.5</v>
+      </c>
+      <c r="O82" s="2">
+        <f t="shared" ref="O82:O85" si="14">SUM(C82+E82)</f>
+        <v>196</v>
+      </c>
+      <c r="P82" s="3" t="str">
+        <f t="shared" ref="P82:P85" si="15">IF(M82&lt;N82,"UNDER","OVER")</f>
+        <v>OVER</v>
+      </c>
+      <c r="Q82" s="2" t="str">
+        <f t="shared" ref="Q82:Q85" si="16">IF(O82&lt;N82,"UNDER","OVER")</f>
+        <v>UNDER</v>
+      </c>
+      <c r="R82" s="2" t="str">
+        <f t="shared" ref="R82:R85" si="17">IF(P82=Q82,"WIN","LOSS")</f>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="2">
+        <v>127</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E83" s="2">
+        <v>121</v>
+      </c>
+      <c r="F83" s="2">
+        <f t="shared" si="12"/>
+        <v>-14</v>
+      </c>
+      <c r="G83" s="2">
+        <v>-9.5</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J83" s="2">
+        <v>92</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L83" s="2">
+        <v>106</v>
+      </c>
+      <c r="M83" s="2">
+        <f t="shared" si="13"/>
+        <v>198</v>
+      </c>
+      <c r="N83" s="2">
+        <v>201.5</v>
+      </c>
+      <c r="O83" s="2">
+        <f t="shared" si="14"/>
+        <v>248</v>
+      </c>
+      <c r="P83" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q83" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>OVER</v>
+      </c>
+      <c r="R83" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84" s="2">
+        <v>89</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E84" s="2">
+        <v>91</v>
+      </c>
+      <c r="F84" s="2">
+        <f t="shared" si="12"/>
+        <v>-4</v>
+      </c>
+      <c r="G84" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J84" s="2">
+        <v>100</v>
+      </c>
+      <c r="K84" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L84" s="2">
+        <v>104</v>
+      </c>
+      <c r="M84" s="2">
+        <f t="shared" si="13"/>
+        <v>204</v>
+      </c>
+      <c r="N84" s="2">
+        <v>202</v>
+      </c>
+      <c r="O84" s="2">
+        <f t="shared" si="14"/>
+        <v>180</v>
+      </c>
+      <c r="P84" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q84" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R84" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>44513</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85" s="2">
+        <v>102</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" s="2">
+        <v>129</v>
+      </c>
+      <c r="F85" s="2">
+        <f t="shared" si="12"/>
+        <v>-12</v>
+      </c>
+      <c r="G85" s="2">
+        <v>-7</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J85" s="2">
+        <v>97</v>
+      </c>
+      <c r="K85" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L85" s="2">
+        <v>109</v>
+      </c>
+      <c r="M85" s="2">
+        <f t="shared" si="13"/>
+        <v>206</v>
+      </c>
+      <c r="N85" s="2">
+        <v>220.5</v>
+      </c>
+      <c r="O85" s="2">
+        <f t="shared" si="14"/>
+        <v>231</v>
+      </c>
+      <c r="P85" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q85" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>OVER</v>
+      </c>
+      <c r="R85" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>LOSS</v>
       </c>
     </row>
   </sheetData>
@@ -6267,27 +6701,27 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>COUNTIF(Archive!$H2:H111,"WIN")</f>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <f>COUNTIF(Archive!$H2:H111,"LOSS")</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C2">
         <f>ROUND(SUM(A2/(A2+B2)),3)</f>
-        <v>0.432</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="D2">
         <f>COUNTIF(Archive!$R2:R111,"WIN")</f>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <f>COUNTIF(Archive!$R2:R111,"LOSS")</f>
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F2">
         <f>ROUND(SUM(D2/(D2+E2)),3)</f>
-        <v>0.49399999999999999</v>
+        <v>0.46400000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated proj. Added confidence games
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735BDC1B-1023-4C5B-8174-ACF2EAB33F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6941EFD-22EF-41D1-BF52-F3FCDF8417EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -230,25 +230,46 @@
     <t>PUSH</t>
   </si>
   <si>
-    <t>San Antonio +2.5</t>
-  </si>
-  <si>
-    <t>Milwaukee +1.5</t>
-  </si>
-  <si>
-    <t>Golden State -5</t>
-  </si>
-  <si>
-    <t>Houston +8.5</t>
-  </si>
-  <si>
-    <t>Oklahoma City +9</t>
-  </si>
-  <si>
-    <t>Portland +6.5</t>
-  </si>
-  <si>
-    <t>Los Angeles Clippers -4</t>
+    <t>Washington -4.5</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>Cleveland +3</t>
+  </si>
+  <si>
+    <t>Sacramento +9</t>
+  </si>
+  <si>
+    <t>Orlando +10.5</t>
+  </si>
+  <si>
+    <t>Indiana +3.5</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>Denver +3.5</t>
+  </si>
+  <si>
+    <t>Houston +11</t>
+  </si>
+  <si>
+    <t>Phoenix -3.5</t>
+  </si>
+  <si>
+    <t>Miami -10</t>
+  </si>
+  <si>
+    <t>Portland -1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los Angeles +1 </t>
   </si>
 </sst>
 </file>
@@ -1154,26 +1175,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.36328125" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.08984375" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="17.36328125" customWidth="1"/>
-    <col min="7" max="7" width="16.26953125" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" customWidth="1"/>
-    <col min="9" max="9" width="14.90625" customWidth="1"/>
+    <col min="2" max="3" width="20.36328125" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.08984375" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+    <col min="9" max="9" width="15.36328125" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" customWidth="1"/>
+    <col min="11" max="11" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1181,228 +1203,416 @@
         <v>61</v>
       </c>
       <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>-2.5</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2">
+        <v>103</v>
+      </c>
+      <c r="H2">
+        <v>201</v>
+      </c>
+      <c r="I2">
+        <v>199.5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>4.5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>110</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>101</v>
+      </c>
+      <c r="H3">
+        <v>211</v>
+      </c>
+      <c r="I3">
+        <v>214.5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>-4.5</v>
+      </c>
+      <c r="B4" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2">
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>96</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4">
+        <v>114</v>
+      </c>
+      <c r="H4">
+        <v>210</v>
+      </c>
+      <c r="I4">
+        <v>207.5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>-10.5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>112</v>
+      </c>
+      <c r="H5">
+        <v>214</v>
+      </c>
+      <c r="I5">
+        <v>214.5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>-3.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>111</v>
+      </c>
+      <c r="H6">
+        <v>220</v>
+      </c>
+      <c r="I6">
+        <v>213</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>-4.5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7">
+        <v>103</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>203</v>
+      </c>
+      <c r="I7">
+        <v>209.5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>-11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8">
         <v>106</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8">
+        <v>108</v>
+      </c>
+      <c r="H8">
+        <v>214</v>
+      </c>
+      <c r="I8">
+        <v>219</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3.5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>111</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <v>101</v>
+      </c>
+      <c r="H9">
+        <v>212</v>
+      </c>
+      <c r="I9">
+        <v>222.5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>98</v>
+      </c>
+      <c r="H10">
+        <v>206</v>
+      </c>
+      <c r="I10">
+        <v>209</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>-1.5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11">
+        <v>111</v>
+      </c>
+      <c r="H11">
+        <v>218</v>
+      </c>
+      <c r="I11">
+        <v>212</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12">
+        <v>106</v>
+      </c>
+      <c r="F12" t="s">
         <v>33</v>
       </c>
-      <c r="F2">
+      <c r="G12">
         <v>107</v>
       </c>
-      <c r="G2">
+      <c r="H12">
         <v>213</v>
       </c>
-      <c r="H2">
-        <v>219.5</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="I12">
+        <v>216.5</v>
+      </c>
+      <c r="J12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>-1.5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <v>111</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3">
-        <v>109</v>
-      </c>
-      <c r="G3">
-        <v>220</v>
-      </c>
-      <c r="H3">
-        <v>221</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4">
-        <v>117</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4">
-        <v>105</v>
-      </c>
-      <c r="G4">
-        <v>222</v>
-      </c>
-      <c r="H4">
-        <v>227</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>8.5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5">
-        <v>110</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5">
-        <v>102</v>
-      </c>
-      <c r="G5">
-        <v>212</v>
-      </c>
-      <c r="H5">
-        <v>221</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6">
-        <v>105</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6">
-        <v>98</v>
-      </c>
-      <c r="G6">
-        <v>203</v>
-      </c>
-      <c r="H6">
-        <v>214.5</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>-6.5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7">
-        <v>102</v>
-      </c>
-      <c r="E7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7">
-        <v>104</v>
-      </c>
-      <c r="G7">
-        <v>206</v>
-      </c>
-      <c r="H7">
-        <v>208</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>-4</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="K12" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8">
-        <v>101</v>
-      </c>
-      <c r="E8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8">
-        <v>109</v>
-      </c>
-      <c r="G8">
-        <v>210</v>
-      </c>
-      <c r="H8">
-        <v>218</v>
-      </c>
-      <c r="I8" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1412,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:R92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6428,7 +6638,7 @@
         <v>92</v>
       </c>
       <c r="F82" s="2">
-        <f t="shared" ref="F82:F85" si="12">SUM(J82 - L82)</f>
+        <f t="shared" ref="F82:F92" si="12">SUM(J82 - L82)</f>
         <v>10</v>
       </c>
       <c r="G82" s="2">
@@ -6450,26 +6660,26 @@
         <v>97</v>
       </c>
       <c r="M82" s="2">
-        <f t="shared" ref="M82:M85" si="13">SUM(J82+L82)</f>
+        <f t="shared" ref="M82:M92" si="13">SUM(J82+L82)</f>
         <v>204</v>
       </c>
       <c r="N82" s="2">
         <v>203.5</v>
       </c>
       <c r="O82" s="2">
-        <f t="shared" ref="O82:O85" si="14">SUM(C82+E82)</f>
+        <f t="shared" ref="O82:O92" si="14">SUM(C82+E82)</f>
         <v>196</v>
       </c>
       <c r="P82" s="3" t="str">
-        <f t="shared" ref="P82:P85" si="15">IF(M82&lt;N82,"UNDER","OVER")</f>
+        <f t="shared" ref="P82:P92" si="15">IF(M82&lt;N82,"UNDER","OVER")</f>
         <v>OVER</v>
       </c>
       <c r="Q82" s="2" t="str">
-        <f t="shared" ref="Q82:Q85" si="16">IF(O82&lt;N82,"UNDER","OVER")</f>
+        <f t="shared" ref="Q82:Q92" si="16">IF(O82&lt;N82,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="R82" s="2" t="str">
-        <f t="shared" ref="R82:R85" si="17">IF(P82=Q82,"WIN","LOSS")</f>
+        <f t="shared" ref="R82:R92" si="17">IF(P82=Q82,"WIN","LOSS")</f>
         <v>LOSS</v>
       </c>
     </row>
@@ -6657,6 +6867,440 @@
       <c r="R85" s="2" t="str">
         <f t="shared" si="17"/>
         <v>LOSS</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C86" s="2">
+        <v>106</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E86" s="2">
+        <v>114</v>
+      </c>
+      <c r="F86" s="2">
+        <f t="shared" si="12"/>
+        <v>-1</v>
+      </c>
+      <c r="G86" s="2">
+        <v>-2.5</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J86" s="2">
+        <v>106</v>
+      </c>
+      <c r="K86" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L86" s="2">
+        <v>107</v>
+      </c>
+      <c r="M86" s="2">
+        <f t="shared" si="13"/>
+        <v>213</v>
+      </c>
+      <c r="N86" s="2">
+        <v>219.5</v>
+      </c>
+      <c r="O86" s="2">
+        <f t="shared" si="14"/>
+        <v>220</v>
+      </c>
+      <c r="P86" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q86" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>OVER</v>
+      </c>
+      <c r="R86" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C87" s="2">
+        <v>100</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E87" s="2">
+        <v>120</v>
+      </c>
+      <c r="F87" s="2">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="G87" s="2">
+        <v>-1.5</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J87" s="2">
+        <v>111</v>
+      </c>
+      <c r="K87" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L87" s="2">
+        <v>109</v>
+      </c>
+      <c r="M87" s="2">
+        <f t="shared" si="13"/>
+        <v>220</v>
+      </c>
+      <c r="N87" s="2">
+        <v>221</v>
+      </c>
+      <c r="O87" s="2">
+        <f t="shared" si="14"/>
+        <v>220</v>
+      </c>
+      <c r="P87" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q87" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R87" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C88" s="2">
+        <v>102</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E88" s="2">
+        <v>106</v>
+      </c>
+      <c r="F88" s="2">
+        <f t="shared" si="12"/>
+        <v>12</v>
+      </c>
+      <c r="G88" s="2">
+        <v>5</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J88" s="2">
+        <v>117</v>
+      </c>
+      <c r="K88" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L88" s="2">
+        <v>105</v>
+      </c>
+      <c r="M88" s="2">
+        <f t="shared" si="13"/>
+        <v>222</v>
+      </c>
+      <c r="N88" s="2">
+        <v>227</v>
+      </c>
+      <c r="O88" s="2">
+        <f t="shared" si="14"/>
+        <v>208</v>
+      </c>
+      <c r="P88" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q88" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R88" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="2">
+        <v>115</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" s="2">
+        <v>89</v>
+      </c>
+      <c r="F89" s="2">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="G89" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J89" s="2">
+        <v>110</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L89" s="2">
+        <v>102</v>
+      </c>
+      <c r="M89" s="2">
+        <f t="shared" si="13"/>
+        <v>212</v>
+      </c>
+      <c r="N89" s="2">
+        <v>221</v>
+      </c>
+      <c r="O89" s="2">
+        <f t="shared" si="14"/>
+        <v>204</v>
+      </c>
+      <c r="P89" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q89" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R89" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>WIN</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90" s="2">
+        <v>120</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E90" s="2">
+        <v>96</v>
+      </c>
+      <c r="F90" s="2">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="G90" s="2">
+        <v>9</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J90" s="2">
+        <v>105</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L90" s="2">
+        <v>98</v>
+      </c>
+      <c r="M90" s="2">
+        <f t="shared" si="13"/>
+        <v>203</v>
+      </c>
+      <c r="N90" s="2">
+        <v>214.5</v>
+      </c>
+      <c r="O90" s="2">
+        <f t="shared" si="14"/>
+        <v>216</v>
+      </c>
+      <c r="P90" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q90" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>OVER</v>
+      </c>
+      <c r="R90" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C91" s="2">
+        <v>95</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E91" s="2">
+        <v>124</v>
+      </c>
+      <c r="F91" s="2">
+        <f t="shared" si="12"/>
+        <v>-2</v>
+      </c>
+      <c r="G91" s="2">
+        <v>-6.5</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J91" s="2">
+        <v>102</v>
+      </c>
+      <c r="K91" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L91" s="2">
+        <v>104</v>
+      </c>
+      <c r="M91" s="2">
+        <f t="shared" si="13"/>
+        <v>206</v>
+      </c>
+      <c r="N91" s="2">
+        <v>208</v>
+      </c>
+      <c r="O91" s="2">
+        <f t="shared" si="14"/>
+        <v>219</v>
+      </c>
+      <c r="P91" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q91" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>OVER</v>
+      </c>
+      <c r="R91" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>LOSS</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>44514</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="2">
+        <v>100</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E92" s="2">
+        <v>90</v>
+      </c>
+      <c r="F92" s="2">
+        <f t="shared" si="12"/>
+        <v>-8</v>
+      </c>
+      <c r="G92" s="2">
+        <v>-4</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J92" s="2">
+        <v>101</v>
+      </c>
+      <c r="K92" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L92" s="2">
+        <v>109</v>
+      </c>
+      <c r="M92" s="2">
+        <f t="shared" si="13"/>
+        <v>210</v>
+      </c>
+      <c r="N92" s="2">
+        <v>218</v>
+      </c>
+      <c r="O92" s="2">
+        <f t="shared" si="14"/>
+        <v>190</v>
+      </c>
+      <c r="P92" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q92" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R92" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>WIN</v>
       </c>
     </row>
   </sheetData>
@@ -6705,23 +7349,23 @@
       </c>
       <c r="B2">
         <f>COUNTIF(Archive!$H2:H111,"LOSS")</f>
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C2">
         <f>ROUND(SUM(A2/(A2+B2)),3)</f>
-        <v>0.45700000000000002</v>
+        <v>0.42</v>
       </c>
       <c r="D2">
         <f>COUNTIF(Archive!$R2:R111,"WIN")</f>
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <f>COUNTIF(Archive!$R2:R111,"LOSS")</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F2">
         <f>ROUND(SUM(D2/(D2+E2)),3)</f>
-        <v>0.46400000000000002</v>
+        <v>0.47299999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update proj.. added injuries in the projection model
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB0041F-8AB7-46AC-A2E7-89EF6DAE38FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88E53BB-C93D-4B26-9E13-6251657A3492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="92">
   <si>
     <t>Date</t>
   </si>
@@ -194,12 +194,6 @@
     <t>Spread Loss</t>
   </si>
   <si>
-    <t>Over Win</t>
-  </si>
-  <si>
-    <t>Over Loss</t>
-  </si>
-  <si>
     <t>NO PLAY</t>
   </si>
   <si>
@@ -239,13 +233,82 @@
     <t>HIGH</t>
   </si>
   <si>
-    <t>Golden State +3</t>
-  </si>
-  <si>
-    <t>Philadelphia +10</t>
-  </si>
-  <si>
     <t>Totals Confidence</t>
+  </si>
+  <si>
+    <t>Washington +1</t>
+  </si>
+  <si>
+    <t>Indiana -1</t>
+  </si>
+  <si>
+    <t>Boston +4.5</t>
+  </si>
+  <si>
+    <t>Cleveland +9.5</t>
+  </si>
+  <si>
+    <t>Chicago +1.5</t>
+  </si>
+  <si>
+    <t>Miami -8</t>
+  </si>
+  <si>
+    <t>New York -12</t>
+  </si>
+  <si>
+    <t>Phoenix -8.5</t>
+  </si>
+  <si>
+    <t>Los Angeles Lakers +9</t>
+  </si>
+  <si>
+    <t>Sacramento +4</t>
+  </si>
+  <si>
+    <t>Houston +2</t>
+  </si>
+  <si>
+    <t>Spread HIGH Win</t>
+  </si>
+  <si>
+    <t>Spread HIGH Loss</t>
+  </si>
+  <si>
+    <t>Spread High Win %</t>
+  </si>
+  <si>
+    <t>Total HIGH Win</t>
+  </si>
+  <si>
+    <t>Totals Win</t>
+  </si>
+  <si>
+    <t>Totals Loss</t>
+  </si>
+  <si>
+    <t>Totals HIGH Loss</t>
+  </si>
+  <si>
+    <t>HIGH %</t>
+  </si>
+  <si>
+    <t>Spread LOW Win</t>
+  </si>
+  <si>
+    <t>Spread LOW Loss</t>
+  </si>
+  <si>
+    <t>Spread LOW Win %</t>
+  </si>
+  <si>
+    <t>Total LOW Win</t>
+  </si>
+  <si>
+    <t>Totals LOW Loss</t>
+  </si>
+  <si>
+    <t>LOW %</t>
   </si>
 </sst>
 </file>
@@ -1151,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1173,13 +1236,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>65</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -1200,115 +1263,395 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E2">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2">
         <v>109</v>
       </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2">
-        <v>102</v>
-      </c>
       <c r="H2">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="I2">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>-10</v>
+        <v>6.5</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="E3">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G3">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="H3">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="I3">
-        <v>216</v>
+        <v>205.5</v>
       </c>
       <c r="J3" t="s">
         <v>31</v>
       </c>
       <c r="K3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>-7.5</v>
+        <v>-4.5</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E4">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="G4">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H4">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="I4">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="J4" t="s">
         <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>-9.5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5">
+        <v>106</v>
+      </c>
+      <c r="H5">
+        <v>204</v>
+      </c>
+      <c r="I5">
+        <v>206</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>-8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6">
+        <v>116</v>
+      </c>
+      <c r="H6">
+        <v>213</v>
+      </c>
+      <c r="I6">
+        <v>213</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>-9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7">
+        <v>108</v>
+      </c>
+      <c r="H7">
+        <v>216</v>
+      </c>
+      <c r="I7">
+        <v>221.5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>-12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8">
+        <v>112</v>
+      </c>
+      <c r="H8">
+        <v>212</v>
+      </c>
+      <c r="I8">
+        <v>208.5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>-2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <v>106</v>
+      </c>
+      <c r="H9">
+        <v>216</v>
+      </c>
+      <c r="I9">
+        <v>227</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>-2.5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10">
+        <v>102</v>
+      </c>
+      <c r="H10">
+        <v>203</v>
+      </c>
+      <c r="I10">
+        <v>213.5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>-8.5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11">
+        <v>96</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11">
+        <v>113</v>
+      </c>
+      <c r="H11">
+        <v>209</v>
+      </c>
+      <c r="I11">
+        <v>212.5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>-1.5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12">
+        <v>107</v>
+      </c>
+      <c r="H12">
+        <v>214</v>
+      </c>
+      <c r="I12">
+        <v>219.5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1318,10 +1661,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R103"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView topLeftCell="C94" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1411,7 +1754,7 @@
         <v>5.5</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>48</v>
@@ -1473,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>39</v>
@@ -1578,7 +1921,7 @@
         <v>44503</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="6">
         <v>98</v>
@@ -1600,7 +1943,7 @@
         <v>20</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J5" s="6">
         <v>102</v>
@@ -1764,7 +2107,7 @@
         <v>44503</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="6">
         <v>106</v>
@@ -1786,7 +2129,7 @@
         <v>20</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J8" s="6">
         <v>90</v>
@@ -1888,7 +2231,7 @@
         <v>44503</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" s="6">
         <v>109</v>
@@ -1910,7 +2253,7 @@
         <v>20</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J10" s="6">
         <v>99</v>
@@ -2918,7 +3261,7 @@
         <v>94</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E27" s="12">
         <v>95</v>
@@ -2940,7 +3283,7 @@
         <v>104</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L27" s="12">
         <v>96</v>
@@ -3042,7 +3385,7 @@
         <v>114</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E29" s="12">
         <v>105</v>
@@ -3064,7 +3407,7 @@
         <v>110</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L29" s="12">
         <v>105</v>
@@ -3104,7 +3447,7 @@
         <v>104</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E30" s="12">
         <v>107</v>
@@ -3126,7 +3469,7 @@
         <v>101</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L30" s="12">
         <v>103</v>
@@ -3848,7 +4191,7 @@
         <v>95</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E42" s="12">
         <v>118</v>
@@ -3870,7 +4213,7 @@
         <v>101</v>
       </c>
       <c r="K42" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L42" s="12">
         <v>107</v>
@@ -3972,7 +4315,7 @@
         <v>92</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E44" s="12">
         <v>108</v>
@@ -3994,7 +4337,7 @@
         <v>106</v>
       </c>
       <c r="K44" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L44" s="12">
         <v>104</v>
@@ -4034,7 +4377,7 @@
         <v>96</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E45" s="12">
         <v>113</v>
@@ -4056,7 +4399,7 @@
         <v>104</v>
       </c>
       <c r="K45" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L45" s="12">
         <v>95</v>
@@ -4772,13 +5115,13 @@
         <v>44510</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C57" s="12">
         <v>107</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E57" s="12">
         <v>117</v>
@@ -4794,13 +5137,13 @@
         <v>20</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J57" s="12">
         <v>100</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L57" s="12">
         <v>107</v>
@@ -5026,7 +5369,7 @@
         <v>98</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E61" s="12">
         <v>101</v>
@@ -5039,7 +5382,7 @@
         <v>3</v>
       </c>
       <c r="H61" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I61" s="12" t="s">
         <v>47</v>
@@ -5048,7 +5391,7 @@
         <v>107</v>
       </c>
       <c r="K61" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L61" s="12">
         <v>96</v>
@@ -5888,7 +6231,7 @@
         <v>44512</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C75" s="12">
         <v>123</v>
@@ -5910,7 +6253,7 @@
         <v>27</v>
       </c>
       <c r="I75" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J75" s="12">
         <v>98</v>
@@ -5956,7 +6299,7 @@
         <v>96</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E76" s="12">
         <v>105</v>
@@ -5978,7 +6321,7 @@
         <v>99</v>
       </c>
       <c r="K76" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L76" s="12">
         <v>109</v>
@@ -6012,7 +6355,7 @@
         <v>44512</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C77" s="12">
         <v>93</v>
@@ -6034,7 +6377,7 @@
         <v>20</v>
       </c>
       <c r="I77" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J77" s="12">
         <v>100</v>
@@ -6334,7 +6677,7 @@
         <v>92</v>
       </c>
       <c r="F82" s="2">
-        <f t="shared" ref="F82:F103" si="12">SUM(J82 - L82)</f>
+        <f t="shared" ref="F82:F106" si="12">SUM(J82 - L82)</f>
         <v>10</v>
       </c>
       <c r="G82" s="2">
@@ -6356,22 +6699,22 @@
         <v>97</v>
       </c>
       <c r="M82" s="2">
-        <f t="shared" ref="M82:M103" si="13">SUM(J82+L82)</f>
+        <f t="shared" ref="M82:M106" si="13">SUM(J82+L82)</f>
         <v>204</v>
       </c>
       <c r="N82" s="2">
         <v>203.5</v>
       </c>
       <c r="O82" s="2">
-        <f t="shared" ref="O82:O103" si="14">SUM(C82+E82)</f>
+        <f t="shared" ref="O82:O106" si="14">SUM(C82+E82)</f>
         <v>196</v>
       </c>
       <c r="P82" s="3" t="str">
-        <f t="shared" ref="P82:P103" si="15">IF(M82&lt;N82,"UNDER","OVER")</f>
+        <f t="shared" ref="P82:P106" si="15">IF(M82&lt;N82,"UNDER","OVER")</f>
         <v>OVER</v>
       </c>
       <c r="Q82" s="2" t="str">
-        <f t="shared" ref="Q82:Q103" si="16">IF(O82&lt;N82,"UNDER","OVER")</f>
+        <f t="shared" ref="Q82:Q106" si="16">IF(O82&lt;N82,"UNDER","OVER")</f>
         <v>UNDER</v>
       </c>
       <c r="R82" s="2" t="str">
@@ -6886,7 +7229,7 @@
         <v>95</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E91" s="2">
         <v>124</v>
@@ -6908,7 +7251,7 @@
         <v>102</v>
       </c>
       <c r="K91" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L91" s="2">
         <v>104</v>
@@ -6942,7 +7285,7 @@
         <v>44514</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C92" s="2">
         <v>100</v>
@@ -6964,7 +7307,7 @@
         <v>27</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J92" s="2">
         <v>101</v>
@@ -7314,13 +7657,13 @@
         <v>44515</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C98" s="2">
         <v>101</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E98" s="2">
         <v>111</v>
@@ -7336,13 +7679,13 @@
         <v>27</v>
       </c>
       <c r="I98" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J98" s="2">
         <v>103</v>
       </c>
       <c r="K98" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L98" s="2">
         <v>100</v>
@@ -7624,7 +7967,7 @@
         <v>44515</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C103" s="2">
         <v>121</v>
@@ -7646,7 +7989,7 @@
         <v>27</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J103" s="2">
         <v>106</v>
@@ -7679,6 +8022,189 @@
       <c r="R103" s="2" t="str">
         <f t="shared" si="17"/>
         <v>LOSS</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A104" s="11">
+        <v>44516</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C104" s="12">
+        <v>117</v>
+      </c>
+      <c r="D104" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E104" s="12">
+        <v>99</v>
+      </c>
+      <c r="F104" s="12">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="G104" s="12">
+        <v>-3</v>
+      </c>
+      <c r="H104" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I104" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J104" s="12">
+        <v>109</v>
+      </c>
+      <c r="K104" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L104" s="12">
+        <v>102</v>
+      </c>
+      <c r="M104" s="12">
+        <f t="shared" si="13"/>
+        <v>211</v>
+      </c>
+      <c r="N104" s="12">
+        <v>222</v>
+      </c>
+      <c r="O104" s="12">
+        <f t="shared" si="14"/>
+        <v>216</v>
+      </c>
+      <c r="P104" s="13" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q104" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R104" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A105" s="11">
+        <v>44516</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C105" s="12">
+        <v>85</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E105" s="12">
+        <v>120</v>
+      </c>
+      <c r="F105" s="12">
+        <f t="shared" si="12"/>
+        <v>-9</v>
+      </c>
+      <c r="G105" s="12">
+        <v>-10</v>
+      </c>
+      <c r="H105" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I105" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J105" s="12">
+        <v>106</v>
+      </c>
+      <c r="K105" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L105" s="12">
+        <v>115</v>
+      </c>
+      <c r="M105" s="12">
+        <f t="shared" si="13"/>
+        <v>221</v>
+      </c>
+      <c r="N105" s="12">
+        <v>216</v>
+      </c>
+      <c r="O105" s="12">
+        <f t="shared" si="14"/>
+        <v>205</v>
+      </c>
+      <c r="P105" s="13" t="str">
+        <f t="shared" si="15"/>
+        <v>OVER</v>
+      </c>
+      <c r="Q105" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R105" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A106" s="11">
+        <v>44516</v>
+      </c>
+      <c r="B106" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C106" s="12">
+        <v>92</v>
+      </c>
+      <c r="D106" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E106" s="12">
+        <v>106</v>
+      </c>
+      <c r="F106" s="12">
+        <f t="shared" si="12"/>
+        <v>-8</v>
+      </c>
+      <c r="G106" s="12">
+        <v>-7.5</v>
+      </c>
+      <c r="H106" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I106" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J106" s="12">
+        <v>101</v>
+      </c>
+      <c r="K106" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="L106" s="12">
+        <v>109</v>
+      </c>
+      <c r="M106" s="12">
+        <f t="shared" si="13"/>
+        <v>210</v>
+      </c>
+      <c r="N106" s="12">
+        <v>220</v>
+      </c>
+      <c r="O106" s="12">
+        <f t="shared" si="14"/>
+        <v>198</v>
+      </c>
+      <c r="P106" s="13" t="str">
+        <f t="shared" si="15"/>
+        <v>UNDER</v>
+      </c>
+      <c r="Q106" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v>UNDER</v>
+      </c>
+      <c r="R106" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -7688,16 +8214,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDBD52-5F97-49F2-81E9-5AECCF07C193}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="3" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -7708,42 +8238,110 @@
         <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>COUNTIF(Archive!$H2:H111,"WIN")</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <f>COUNTIF(Archive!$H2:H111,"LOSS")</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <f>ROUND(SUM(A2/(A2+B2)),3)</f>
-        <v>0.41399999999999998</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="D2">
         <f>COUNTIF(Archive!$R2:R111,"WIN")</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2">
         <f>COUNTIF(Archive!$R2:R111,"LOSS")</f>
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2">
         <f>ROUND(SUM(D2/(D2+E2)),3)</f>
-        <v>0.45100000000000001</v>
+        <v>0.45700000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update kevin durant inury for 11/19/2021
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5EC392-E21A-4BF3-92A3-C9333F4F36C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7006E02D-DBEC-4F1E-B61E-07FB0632208E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -281,9 +281,6 @@
     <t>Charlotte -2</t>
   </si>
   <si>
-    <t>Brooklyn -12.5</t>
-  </si>
-  <si>
     <t>Sacramento -3.5</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>Phoenix - 8.5</t>
+  </si>
+  <si>
+    <t>Orlando +10</t>
   </si>
 </sst>
 </file>
@@ -1210,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1304,7 +1304,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
@@ -1339,7 +1339,7 @@
         <v>-2</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -1371,13 +1371,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>-12.5</v>
+        <v>-10</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
@@ -1389,10 +1389,10 @@
         <v>34</v>
       </c>
       <c r="G5">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H5">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I5">
         <v>214.5</v>
@@ -1409,7 +1409,7 @@
         <v>-12.5</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -1444,7 +1444,7 @@
         <v>3.5</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
@@ -1479,7 +1479,7 @@
         <v>-3</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
@@ -1514,7 +1514,7 @@
         <v>-8.5</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>65</v>
@@ -1549,7 +1549,7 @@
         <v>-3.5</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
         <v>65</v>
@@ -9195,7 +9195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDBD52-5F97-49F2-81E9-5AECCF07C193}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update proj steph curry out
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7006E02D-DBEC-4F1E-B61E-07FB0632208E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F4D41F-179E-4EDB-9BC8-B1DFD3BE2CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -284,9 +284,6 @@
     <t>Sacramento -3.5</t>
   </si>
   <si>
-    <t>Golden State - 7</t>
-  </si>
-  <si>
     <t>Los Angeles Lakers +2</t>
   </si>
   <si>
@@ -303,6 +300,9 @@
   </si>
   <si>
     <t>Orlando +10</t>
+  </si>
+  <si>
+    <t>Golden State - 2</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1301,10 +1301,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>
@@ -1313,7 +1313,7 @@
         <v>46</v>
       </c>
       <c r="E3">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -1322,16 +1322,16 @@
         <v>91</v>
       </c>
       <c r="H3">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="I3">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1339,7 +1339,7 @@
         <v>-2</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -1374,7 +1374,7 @@
         <v>-10</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
@@ -1409,7 +1409,7 @@
         <v>-12.5</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -1444,7 +1444,7 @@
         <v>3.5</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
@@ -1479,7 +1479,7 @@
         <v>-3</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
         <v>64</v>
@@ -1514,7 +1514,7 @@
         <v>-8.5</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
update anthony davis injury
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF0BDAC-DF80-4159-BC92-456A8FF787C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE33B25-2E94-4A3E-AAF4-F7574B7C1AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>NONE</t>
-  </si>
-  <si>
-    <t>Los Angeles Lakers +5.5</t>
   </si>
   <si>
     <t>Houston +10</t>
@@ -1207,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1301,16 +1298,16 @@
         <v>-5.5</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
       </c>
       <c r="E3">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F3" t="s">
         <v>47</v>
@@ -1319,16 +1316,16 @@
         <v>109</v>
       </c>
       <c r="H3">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="I3">
-        <v>217</v>
+        <v>216.5</v>
       </c>
       <c r="J3" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1406,7 +1403,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
         <v>64</v>
@@ -1546,7 +1543,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
         <v>64</v>
@@ -1616,7 +1613,7 @@
         <v>3.5</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -1651,7 +1648,7 @@
         <v>-10.5</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
         <v>65</v>
@@ -11542,7 +11539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19BDBD52-5F97-49F2-81E9-5AECCF07C193}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nets updated line with harden out
</commit_message>
<xml_diff>
--- a/UpdatedResults.xlsx
+++ b/UpdatedResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NBA-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C168F2F1-56C9-49DB-9128-194CBD8F07B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA7BAB4-41B0-4C43-8E69-38A61E9F047B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-1050" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedResults" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -285,9 +285,6 @@
   </si>
   <si>
     <t>NONE</t>
-  </si>
-  <si>
-    <t>Brooklyn -5</t>
   </si>
   <si>
     <t>Golden State -5</t>
@@ -1205,7 +1202,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1263,10 +1260,10 @@
         <v>-5</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>42</v>
@@ -1281,16 +1278,16 @@
         <v>111</v>
       </c>
       <c r="H2">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="I2">
         <v>216</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -1298,7 +1295,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -1333,7 +1330,7 @@
         <v>1.5</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>

</xml_diff>